<commit_message>
Txt file of prefers
</commit_message>
<xml_diff>
--- a/Planilha.xlsx
+++ b/Planilha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tulio\Desktop\-\Programação\Projetos programação\Horarios-CEFET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904EE22D-1DCF-4D6E-BD95-489C77757124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1D2834-DBFB-4A7D-B728-B8B452F82BCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>Professor</t>
   </si>
@@ -140,6 +140,36 @@
   </si>
   <si>
     <t>S3-N5-N6</t>
+  </si>
+  <si>
+    <t>Programação</t>
+  </si>
+  <si>
+    <t>MTRM</t>
+  </si>
+  <si>
+    <t>Pedro Francisco</t>
+  </si>
+  <si>
+    <t>Sistemas digitais</t>
+  </si>
+  <si>
+    <t>Lucas Ferreira</t>
+  </si>
+  <si>
+    <t>S2-N5</t>
+  </si>
+  <si>
+    <t>Motores de aplicação</t>
+  </si>
+  <si>
+    <t>Jorge Aquino</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>N6</t>
   </si>
 </sst>
 </file>
@@ -502,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,6 +596,9 @@
       <c r="H2">
         <v>2</v>
       </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -812,6 +845,104 @@
         <v>1</v>
       </c>
       <c r="H12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prefers update and making it work
</commit_message>
<xml_diff>
--- a/Planilha.xlsx
+++ b/Planilha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tulio\Desktop\-\Programação\Projetos programação\Horarios-CEFET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45562D1E-025F-4103-900E-9E5B5725A403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F37597A-E85F-4550-B82C-2B65F9EBF734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Professor</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>S5:2,3</t>
+  </si>
+  <si>
+    <t>N2:1,3</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +813,7 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="H9">
         <v>2</v>

</xml_diff>